<commit_message>
feat: add Excel and SQL practice files
Add new Excel workbooks and SQL practice file with employee table creation and sample data
</commit_message>
<xml_diff>
--- a/Excel_PowerBI/Excel_Day_1.xlsx
+++ b/Excel_PowerBI/Excel_Day_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohit\Documents\Projects\Pyspiders\Excel_PowerBI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D69787F-7367-48AC-AA02-D3CC5EB30937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F35A26F-1D28-4896-A525-3967A3C570C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4A693938-57C8-4F3F-B118-A0A45FC2C460}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Science</t>
   </si>
@@ -76,16 +76,55 @@
   </si>
   <si>
     <t>Rashad</t>
+  </si>
+  <si>
+    <t>Gopi</t>
+  </si>
+  <si>
+    <t>Dhanush</t>
+  </si>
+  <si>
+    <t>Dharshan</t>
+  </si>
+  <si>
+    <t>Vijay</t>
+  </si>
+  <si>
+    <t>Sunil</t>
+  </si>
+  <si>
+    <t>Ajith</t>
+  </si>
+  <si>
+    <t>Sanjay</t>
+  </si>
+  <si>
+    <t>Hari</t>
+  </si>
+  <si>
+    <t>Goplan</t>
+  </si>
+  <si>
+    <t>Veerash</t>
+  </si>
+  <si>
+    <t>Soma</t>
+  </si>
+  <si>
+    <t>Naveen</t>
+  </si>
+  <si>
+    <t>Praveen</t>
+  </si>
+  <si>
+    <t>Pramith</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="_ [$₹-4009]\ * #,##0.00_ ;_ [$₹-4009]\ * \-#,##0.00_ ;_ [$₹-4009]\ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +138,13 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -127,24 +173,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -460,25 +511,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E260474-EB8D-4466-95CF-898163335926}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -503,8 +554,23 @@
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -512,25 +578,46 @@
         <v>8</v>
       </c>
       <c r="C2" s="3">
-        <v>94</v>
+        <f ca="1">RANDBETWEEN(10,100)</f>
+        <v>16</v>
       </c>
       <c r="D2" s="3">
-        <v>78</v>
+        <f t="shared" ref="D2:H17" ca="1" si="0">RANDBETWEEN(10,100)</f>
+        <v>62</v>
       </c>
       <c r="E2" s="3">
-        <v>39</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
       </c>
       <c r="F2" s="3">
-        <v>93</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
       </c>
       <c r="G2" s="3">
-        <v>95</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
       </c>
       <c r="H2" s="3">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -538,25 +625,46 @@
         <v>9</v>
       </c>
       <c r="C3" s="3">
-        <v>56</v>
+        <f t="shared" ref="C3:H21" ca="1" si="1">RANDBETWEEN(10,100)</f>
+        <v>41</v>
       </c>
       <c r="D3" s="3">
-        <v>80</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>53</v>
       </c>
       <c r="E3" s="3">
-        <v>75</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
       </c>
       <c r="F3" s="3">
-        <v>67</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>79</v>
       </c>
       <c r="G3" s="3">
-        <v>98</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
       </c>
       <c r="H3" s="3">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -564,25 +672,46 @@
         <v>10</v>
       </c>
       <c r="C4" s="3">
-        <v>40</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>61</v>
       </c>
       <c r="D4" s="3">
-        <v>62</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>65</v>
       </c>
       <c r="E4" s="3">
-        <v>79</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>73</v>
       </c>
       <c r="F4" s="3">
-        <v>54</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
       </c>
       <c r="G4" s="3">
-        <v>99</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>49</v>
       </c>
       <c r="H4" s="3">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -590,25 +719,46 @@
         <v>11</v>
       </c>
       <c r="C5" s="3">
-        <v>64</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>68</v>
       </c>
       <c r="D5" s="3">
-        <v>41</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>54</v>
       </c>
       <c r="E5" s="3">
-        <v>100</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>38</v>
       </c>
       <c r="F5" s="3">
-        <v>94</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>34</v>
       </c>
       <c r="G5" s="3">
-        <v>42</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
       </c>
       <c r="H5" s="3">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -616,25 +766,46 @@
         <v>12</v>
       </c>
       <c r="C6" s="3">
-        <v>38</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>35</v>
       </c>
       <c r="D6" s="3">
-        <v>88</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
       </c>
       <c r="E6" s="3">
-        <v>47</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>65</v>
       </c>
       <c r="F6" s="3">
-        <v>39</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
       </c>
       <c r="G6" s="3">
-        <v>73</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>74</v>
       </c>
       <c r="H6" s="3">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -642,360 +813,708 @@
         <v>13</v>
       </c>
       <c r="C7" s="3">
-        <v>35</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>73</v>
       </c>
       <c r="D7" s="3">
-        <v>65</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>41</v>
       </c>
       <c r="E7" s="3">
-        <v>89</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
       </c>
       <c r="F7" s="3">
-        <v>77</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
       </c>
       <c r="G7" s="3">
-        <v>87</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>83</v>
       </c>
       <c r="H7" s="3">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="C8" s="3">
-        <v>82</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>72</v>
       </c>
       <c r="D8" s="3">
-        <v>69</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>80</v>
       </c>
       <c r="E8" s="3">
-        <v>35</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>67</v>
       </c>
       <c r="F8" s="3">
-        <v>94</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
       </c>
       <c r="G8" s="3">
-        <v>88</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>55</v>
       </c>
       <c r="H8" s="3">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="C9" s="3">
-        <v>69</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>47</v>
       </c>
       <c r="D9" s="3">
-        <v>78</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
       </c>
       <c r="E9" s="3">
-        <v>44</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
       </c>
       <c r="F9" s="3">
-        <v>48</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
       </c>
       <c r="G9" s="3">
-        <v>92</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>35</v>
       </c>
       <c r="H9" s="3">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="C10" s="3">
-        <v>69</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>40</v>
       </c>
       <c r="D10" s="3">
-        <v>77</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>89</v>
       </c>
       <c r="E10" s="3">
-        <v>42</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>38</v>
       </c>
       <c r="F10" s="3">
-        <v>97</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
       </c>
       <c r="G10" s="3">
-        <v>75</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
       </c>
       <c r="H10" s="3">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="C11" s="3">
-        <v>57</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>80</v>
       </c>
       <c r="D11" s="3">
-        <v>74</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
       </c>
       <c r="E11" s="3">
-        <v>68</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>54</v>
       </c>
       <c r="F11" s="3">
-        <v>89</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>32</v>
       </c>
       <c r="G11" s="3">
-        <v>73</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
       </c>
       <c r="H11" s="3">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="C12" s="3">
-        <v>96</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43</v>
       </c>
       <c r="D12" s="3">
-        <v>55</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
       </c>
       <c r="E12" s="3">
-        <v>79</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>59</v>
       </c>
       <c r="F12" s="3">
-        <v>73</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
       </c>
       <c r="G12" s="3">
-        <v>35.999899999999997</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>82</v>
       </c>
       <c r="H12" s="3">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="7"/>
+      <c r="B13" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="C13" s="3">
-        <v>76</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>95</v>
       </c>
       <c r="D13" s="3">
-        <v>89</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>73</v>
       </c>
       <c r="E13" s="3">
-        <v>54</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
       </c>
       <c r="F13" s="3">
-        <v>83</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45</v>
       </c>
       <c r="G13" s="3">
-        <v>43</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>57</v>
       </c>
       <c r="H13" s="3">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="C14" s="3">
-        <v>100</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>85</v>
       </c>
       <c r="D14" s="3">
-        <v>64</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>71</v>
       </c>
       <c r="E14" s="3">
-        <v>86</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>65</v>
       </c>
       <c r="F14" s="3">
-        <v>45</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>81</v>
       </c>
       <c r="G14" s="3">
-        <v>86</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>18</v>
       </c>
       <c r="H14" s="3">
-        <v>65</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>41</v>
       </c>
       <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14" s="6"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="C15" s="3">
-        <v>68</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>80</v>
       </c>
       <c r="D15" s="3">
-        <v>48</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
       </c>
       <c r="E15" s="3">
-        <v>41</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>83</v>
       </c>
       <c r="F15" s="3">
-        <v>57</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
       </c>
       <c r="G15" s="3">
-        <v>50</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
       </c>
       <c r="H15" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="C16" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" ca="1" si="0"/>
         <v>62</v>
       </c>
-      <c r="D16" s="3">
+      <c r="G16" s="3">
+        <f t="shared" ca="1" si="0"/>
         <v>88</v>
       </c>
-      <c r="E16" s="3">
-        <v>69</v>
-      </c>
-      <c r="F16" s="3">
-        <v>43</v>
-      </c>
-      <c r="G16" s="3">
-        <v>83</v>
-      </c>
       <c r="H16" s="3">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="C17" s="3">
-        <v>59</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>46</v>
       </c>
       <c r="D17" s="3">
-        <v>93</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>33</v>
       </c>
       <c r="E17" s="3">
-        <v>93</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>71</v>
       </c>
       <c r="F17" s="3">
-        <v>95</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>71</v>
       </c>
       <c r="G17" s="3">
-        <v>60</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>69</v>
       </c>
       <c r="H17" s="3">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="5"/>
+      <c r="B18" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="C18" s="3">
-        <v>36</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>60</v>
       </c>
       <c r="D18" s="3">
-        <v>96</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>65</v>
       </c>
       <c r="E18" s="3">
-        <v>80</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>84</v>
       </c>
       <c r="F18" s="3">
-        <v>73</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>76</v>
       </c>
       <c r="G18" s="3">
-        <v>100</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>33</v>
       </c>
       <c r="H18" s="3">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="5"/>
+      <c r="B19" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="C19" s="3">
-        <v>58</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>56</v>
       </c>
       <c r="D19" s="3">
-        <v>64</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
       </c>
       <c r="E19" s="3">
-        <v>61</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>78</v>
       </c>
       <c r="F19" s="3">
-        <v>64</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>55</v>
       </c>
       <c r="G19" s="3">
-        <v>44</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>69</v>
       </c>
       <c r="H19" s="3">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="5"/>
+      <c r="B20" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="C20" s="3">
-        <v>46</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>85</v>
       </c>
       <c r="D20" s="3">
-        <v>42</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>13</v>
       </c>
       <c r="E20" s="3">
-        <v>98</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>47</v>
       </c>
       <c r="F20" s="3">
-        <v>61</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
       </c>
       <c r="G20" s="3">
-        <v>80</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>82</v>
       </c>
       <c r="H20" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="5"/>
+      <c r="B21" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="C21" s="3">
-        <v>82</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>52</v>
       </c>
       <c r="D21" s="3">
-        <v>67</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
       </c>
       <c r="E21" s="3">
-        <v>49</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>56</v>
       </c>
       <c r="F21" s="3">
-        <v>44</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>13</v>
       </c>
       <c r="G21" s="3">
+        <f t="shared" ca="1" si="1"/>
         <v>71</v>
       </c>
       <c r="H21" s="3">
-        <v>54</v>
-      </c>
+        <f t="shared" ca="1" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="K23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>